<commit_message>
Ficha educatico sub categorias de vida estudiantil
Se completa las fichas e subcategorias de vida estudiantil para la subida a educatico
</commit_message>
<xml_diff>
--- a/documentacion/vidaestudiantil/Subida a Educatico/ficha_educatico-AGENDAESTUDIANTL-SUBCATEGORIAS.xlsx
+++ b/documentacion/vidaestudiantil/Subida a Educatico/ficha_educatico-AGENDAESTUDIANTL-SUBCATEGORIAS.xlsx
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="213">
   <si>
     <t>Título</t>
   </si>
@@ -823,9 +823,6 @@
   </si>
   <si>
     <t>Ciencias Sociales-Grupos Sociales</t>
-  </si>
-  <si>
-    <t>GESPRO SE ENCARGA DE TRÁMITARLA</t>
   </si>
   <si>
     <t>Todas</t>
@@ -1578,13 +1575,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1596,43 +1623,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1721,6 +1718,239 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>607219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1383277</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1430840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22145624" y="1095375"/>
+          <a:ext cx="1252309" cy="823621"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>130968</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1569698</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1004598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22228969" y="3047999"/>
+          <a:ext cx="1355385" cy="873630"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>229093</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1610169</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1012031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22243749" y="4167187"/>
+          <a:ext cx="1381076" cy="869157"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>110184</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>547687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1714054</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>449775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22124840" y="5679281"/>
+          <a:ext cx="1603870" cy="1009369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>71439</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>404814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12723</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22086095" y="7750970"/>
+          <a:ext cx="1655784" cy="1083468"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>250031</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>35267</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>285445</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22061581" y="12025312"/>
+          <a:ext cx="1702842" cy="1142696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2012,19 +2242,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="I8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.28515625" style="29" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="29" hidden="1" customWidth="1"/>
-    <col min="3" max="7" width="25.7109375" style="29" hidden="1" customWidth="1"/>
-    <col min="8" max="10" width="20.7109375" style="29" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="29" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="29" customWidth="1"/>
+    <col min="3" max="7" width="25.7109375" style="29" customWidth="1"/>
+    <col min="8" max="10" width="20.7109375" style="29" customWidth="1"/>
+    <col min="11" max="11" width="20" style="29" customWidth="1"/>
     <col min="12" max="12" width="40.85546875" style="42" customWidth="1"/>
-    <col min="13" max="13" width="25.7109375" style="42" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" style="42" customWidth="1"/>
     <col min="14" max="14" width="25.7109375" style="29" customWidth="1"/>
     <col min="15" max="16" width="20.7109375" style="29" customWidth="1"/>
     <col min="17" max="17" width="25.7109375" style="33" customWidth="1"/>
@@ -2032,24 +2262,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
       <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -2102,21 +2332,21 @@
         <v>6</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>159</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>163</v>
@@ -2139,14 +2369,12 @@
       <c r="K3" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="L3" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>167</v>
-      </c>
+      <c r="L3" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="M3" s="37"/>
       <c r="N3" s="36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -2155,16 +2383,16 @@
     </row>
     <row r="4" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>159</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>163</v>
@@ -2182,19 +2410,17 @@
         <v>164</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K4" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="L4" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="M4" s="37" t="s">
-        <v>167</v>
-      </c>
+      <c r="L4" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="37"/>
       <c r="N4" s="36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
@@ -2203,16 +2429,16 @@
     </row>
     <row r="5" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>159</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>163</v>
@@ -2235,14 +2461,12 @@
       <c r="K5" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="L5" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="M5" s="37" t="s">
-        <v>167</v>
-      </c>
+      <c r="L5" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5" s="37"/>
       <c r="N5" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
@@ -2250,47 +2474,45 @@
       <c r="R5" s="6"/>
     </row>
     <row r="6" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="H6" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="J6" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="L6" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="53" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>160</v>
-      </c>
-      <c r="I6" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="J6" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="K6" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="L6" s="50" t="s">
-        <v>180</v>
-      </c>
-      <c r="M6" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="N6" s="59" t="s">
-        <v>213</v>
+      <c r="M6" s="59"/>
+      <c r="N6" s="47" t="s">
+        <v>212</v>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="41"/>
@@ -2298,71 +2520,69 @@
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="54" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="50" t="s">
+      <c r="A7" s="54"/>
+      <c r="B7" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="56"/>
-      <c r="N7" s="60"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="M7" s="61"/>
+      <c r="N7" s="48"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="39"/>
       <c r="R7" s="6"/>
     </row>
     <row r="8" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" s="43" t="s">
+      <c r="D8" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="I8" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="J8" s="43" t="s">
+      <c r="I8" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="J8" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="K8" s="43" t="s">
+      <c r="K8" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="L8" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="M8" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="N8" s="59" t="s">
-        <v>212</v>
+      <c r="L8" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="M8" s="59"/>
+      <c r="N8" s="47" t="s">
+        <v>211</v>
       </c>
       <c r="O8" s="41"/>
       <c r="P8" s="41"/>
@@ -2370,69 +2590,67 @@
       <c r="R8" s="6"/>
     </row>
     <row r="9" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="50" t="s">
-        <v>210</v>
-      </c>
-      <c r="M9" s="56"/>
-      <c r="N9" s="60"/>
+        <v>186</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="M9" s="61"/>
+      <c r="N9" s="48"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="40"/>
       <c r="R9" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
-        <v>188</v>
+      <c r="A10" s="53" t="s">
+        <v>187</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" s="43" t="s">
+      <c r="D10" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="I10" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43" t="s">
+      <c r="I10" s="50" t="s">
+        <v>204</v>
+      </c>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="L10" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="M10" s="55" t="s">
-        <v>167</v>
-      </c>
-      <c r="N10" s="59" t="s">
-        <v>211</v>
+      <c r="L10" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="M10" s="59"/>
+      <c r="N10" s="47" t="s">
+        <v>210</v>
       </c>
       <c r="O10" s="41"/>
       <c r="P10" s="41"/>
@@ -2440,168 +2658,168 @@
       <c r="R10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="50" t="s">
-        <v>191</v>
-      </c>
-      <c r="M11" s="58"/>
-      <c r="N11" s="61"/>
+        <v>197</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="M11" s="60"/>
+      <c r="N11" s="49"/>
       <c r="O11" s="41"/>
       <c r="P11" s="41"/>
       <c r="Q11" s="40"/>
       <c r="R11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="50" t="s">
-        <v>192</v>
-      </c>
-      <c r="M12" s="58"/>
-      <c r="N12" s="61"/>
+        <v>198</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="M12" s="60"/>
+      <c r="N12" s="49"/>
       <c r="O12" s="41"/>
       <c r="P12" s="41"/>
       <c r="Q12" s="40"/>
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="50" t="s">
-        <v>193</v>
-      </c>
-      <c r="M13" s="58"/>
-      <c r="N13" s="61"/>
+        <v>199</v>
+      </c>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="M13" s="60"/>
+      <c r="N13" s="49"/>
       <c r="O13" s="41"/>
       <c r="P13" s="41"/>
       <c r="Q13" s="40"/>
       <c r="R13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="41" t="s">
-        <v>201</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="M14" s="58"/>
-      <c r="N14" s="61"/>
+        <v>200</v>
+      </c>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="M14" s="60"/>
+      <c r="N14" s="49"/>
       <c r="O14" s="41"/>
       <c r="P14" s="41"/>
       <c r="Q14" s="40"/>
       <c r="R14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="M15" s="58"/>
-      <c r="N15" s="61"/>
+        <v>201</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="M15" s="60"/>
+      <c r="N15" s="49"/>
       <c r="O15" s="41"/>
       <c r="P15" s="41"/>
       <c r="Q15" s="40"/>
       <c r="R15" s="6"/>
     </row>
     <row r="16" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="57"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="50" t="s">
-        <v>195</v>
-      </c>
-      <c r="M16" s="58"/>
-      <c r="N16" s="61"/>
+        <v>202</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="M16" s="60"/>
+      <c r="N16" s="49"/>
       <c r="O16" s="41"/>
       <c r="P16" s="41"/>
       <c r="Q16" s="40"/>
       <c r="R16" s="6"/>
     </row>
     <row r="17" spans="1:18" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="M17" s="56"/>
-      <c r="N17" s="60"/>
+        <v>203</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="M17" s="61"/>
+      <c r="N17" s="48"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="40"/>
@@ -2609,30 +2827,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N10:N17"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="E10:E17"/>
-    <mergeCell ref="F10:F17"/>
-    <mergeCell ref="G10:G17"/>
-    <mergeCell ref="H10:H17"/>
-    <mergeCell ref="I10:I17"/>
-    <mergeCell ref="J10:J17"/>
-    <mergeCell ref="K10:K17"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="C10:C17"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
@@ -2641,10 +2835,34 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="E10:E17"/>
+    <mergeCell ref="F10:F17"/>
+    <mergeCell ref="G10:G17"/>
+    <mergeCell ref="H10:H17"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N10:N17"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I10:I17"/>
+    <mergeCell ref="J10:J17"/>
+    <mergeCell ref="K10:K17"/>
     <mergeCell ref="M10:M17"/>
-    <mergeCell ref="M6:M7"/>
     <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K6:K7"/>
     <mergeCell ref="N8:N9"/>
   </mergeCells>
   <hyperlinks>
@@ -2670,7 +2888,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Predeterminado"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Predeterminado"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId17"/>
+  <drawing r:id="rId17"/>
+  <legacyDrawing r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>